<commit_message>
Exception handling in get_f1_score for TextRank
</commit_message>
<xml_diff>
--- a/Evaluation.xlsx
+++ b/Evaluation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Sem VII\Final Year Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Sem VII\Final Year Project\FYP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CB4AE6-5212-4624-88A3-F87D7BA0454B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE746F7-5E6A-4871-9F78-B9B8971E33D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5724" yWindow="2556" windowWidth="16584" windowHeight="9420" xr2:uid="{27D1B984-DA68-464F-8F8A-D4BB6C213CE9}"/>
+    <workbookView xWindow="11304" yWindow="5124" windowWidth="16584" windowHeight="9420" xr2:uid="{27D1B984-DA68-464F-8F8A-D4BB6C213CE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
   <si>
     <t>Word Frequency</t>
   </si>
@@ -51,6 +51,18 @@
   </si>
   <si>
     <t>chandrayaan</t>
+  </si>
+  <si>
+    <t>TextRank</t>
+  </si>
+  <si>
+    <t>iphone</t>
+  </si>
+  <si>
+    <t>turkey</t>
+  </si>
+  <si>
+    <t>microsoft</t>
   </si>
 </sst>
 </file>
@@ -168,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -187,6 +199,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{325B10D9-10B0-4F88-913C-29C91C62F312}">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28:F28"/>
+    <sheetView tabSelected="1" topLeftCell="B55" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -815,6 +831,9 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
       <c r="D25" s="3">
         <v>8.3999999999999995E-3</v>
       </c>
@@ -826,6 +845,9 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
       <c r="D26" s="5">
         <v>1.4500000000000001E-2</v>
       </c>
@@ -837,6 +859,9 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
       <c r="D27" s="5">
         <v>0.2109</v>
       </c>
@@ -1085,7 +1110,7 @@
         <v>0.40450000000000003</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D49">
         <v>0.3291</v>
       </c>
@@ -1096,7 +1121,7 @@
         <v>0.42280000000000001</v>
       </c>
     </row>
-    <row r="50" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D50" s="1">
         <f>AVERAGE(D47:D49)</f>
         <v>0.35786666666666661</v>
@@ -1110,7 +1135,7 @@
         <v>0.44693333333333335</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>6</v>
       </c>
@@ -1124,7 +1149,7 @@
         <v>0.55320000000000003</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D52">
         <v>0.1515</v>
       </c>
@@ -1135,7 +1160,7 @@
         <v>0.16259999999999999</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D53">
         <v>0.20580000000000001</v>
       </c>
@@ -1146,7 +1171,7 @@
         <v>0.27450000000000002</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D54">
         <v>0.25</v>
       </c>
@@ -1157,7 +1182,7 @@
         <v>0.23730000000000001</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D55">
         <v>0.25490000000000002</v>
       </c>
@@ -1168,7 +1193,7 @@
         <v>0.1978</v>
       </c>
     </row>
-    <row r="56" spans="2:6" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D56" s="1">
         <f>AVERAGE(D51:D55)</f>
         <v>0.25122</v>
@@ -1182,7 +1207,10 @@
         <v>0.28508</v>
       </c>
     </row>
-    <row r="57" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B57" t="s">
+        <v>8</v>
+      </c>
       <c r="D57" s="3">
         <v>0.1056</v>
       </c>
@@ -1193,7 +1221,10 @@
         <v>0.1109</v>
       </c>
     </row>
-    <row r="58" spans="2:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B58" t="s">
+        <v>10</v>
+      </c>
       <c r="D58" s="5">
         <v>0.16830000000000001</v>
       </c>
@@ -1204,7 +1235,10 @@
         <v>0.21840000000000001</v>
       </c>
     </row>
-    <row r="59" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B59" t="s">
+        <v>9</v>
+      </c>
       <c r="D59" s="5">
         <v>0.31040000000000001</v>
       </c>
@@ -1215,7 +1249,7 @@
         <v>0.33800000000000002</v>
       </c>
     </row>
-    <row r="60" spans="2:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D60" s="2">
         <f>AVERAGE(D36,D42,D46,D50,D56,D57:D59)</f>
         <v>0.23796024999999998</v>
@@ -1227,6 +1261,209 @@
       <c r="F60" s="2">
         <f t="shared" si="5"/>
         <v>0.27313999999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1</v>
+      </c>
+      <c r="D62" s="8">
+        <v>0.26519999999999999</v>
+      </c>
+      <c r="E62" s="9">
+        <v>0.2581</v>
+      </c>
+      <c r="F62" s="9">
+        <v>0.2616</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D63">
+        <v>8.6400000000000005E-2</v>
+      </c>
+      <c r="E63">
+        <v>0.36359999999999998</v>
+      </c>
+      <c r="F63">
+        <v>0.1396</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D64" s="1">
+        <f>AVERAGE(D62:D63)</f>
+        <v>0.17580000000000001</v>
+      </c>
+      <c r="E64" s="1">
+        <f t="shared" ref="E64:F64" si="6">AVERAGE(E62:E63)</f>
+        <v>0.31084999999999996</v>
+      </c>
+      <c r="F64" s="1">
+        <f t="shared" si="6"/>
+        <v>0.2006</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D65">
+        <v>1.8200000000000001E-2</v>
+      </c>
+      <c r="E65">
+        <v>3.4500000000000003E-2</v>
+      </c>
+      <c r="F65">
+        <v>2.3800000000000002E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D66">
+        <v>0.1298</v>
+      </c>
+      <c r="E66">
+        <v>0.35070000000000001</v>
+      </c>
+      <c r="F66">
+        <v>0.1895</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D67">
+        <v>0.1923</v>
+      </c>
+      <c r="E67">
+        <v>0.625</v>
+      </c>
+      <c r="F67">
+        <v>0.29411700000000002</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D68">
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="E68">
+        <v>4.050405E-2</v>
+      </c>
+      <c r="F68">
+        <v>4.054E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D69" s="1">
+        <f>AVERAGE(D65:D68)</f>
+        <v>0.18642500000000001</v>
+      </c>
+      <c r="E69" s="1">
+        <f t="shared" ref="E69:F69" si="7">AVERAGE(E65:E68)</f>
+        <v>0.2626760125</v>
+      </c>
+      <c r="F69" s="1">
+        <f t="shared" si="7"/>
+        <v>0.13698925000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>4</v>
+      </c>
+      <c r="D70">
+        <v>0.29729</v>
+      </c>
+      <c r="E70">
+        <v>0.49253000000000002</v>
+      </c>
+      <c r="F70">
+        <v>0.37078</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D71">
+        <v>0.30908999999999998</v>
+      </c>
+      <c r="E71">
+        <v>0.31774999999999998</v>
+      </c>
+      <c r="F71">
+        <v>0.31336399999999998</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D72" s="1">
+        <f>AVERAGE(D70:D71)</f>
+        <v>0.30318999999999996</v>
+      </c>
+      <c r="E72" s="1">
+        <f t="shared" ref="E72:F72" si="8">AVERAGE(E70:E71)</f>
+        <v>0.40514</v>
+      </c>
+      <c r="F72" s="1">
+        <f t="shared" si="8"/>
+        <v>0.34207199999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73">
+        <v>0.21679899999999999</v>
+      </c>
+      <c r="E73">
+        <v>0.33567000000000002</v>
+      </c>
+      <c r="F73">
+        <v>0.26344800000000002</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D74">
+        <v>0.13216900000000001</v>
+      </c>
+      <c r="E74">
+        <v>0.28494000000000003</v>
+      </c>
+      <c r="F74">
+        <v>0.18057899999999999</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D75">
+        <v>0.33082699999999998</v>
+      </c>
+      <c r="E75">
+        <v>0.90720999999999996</v>
+      </c>
+      <c r="F75">
+        <v>0.484848</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D76">
+        <v>0.22792000000000001</v>
+      </c>
+      <c r="E76">
+        <v>0.21276</v>
+      </c>
+      <c r="F76">
+        <v>0.22008249999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D77" s="1">
+        <f>AVERAGE(D73:D76)</f>
+        <v>0.22692874999999998</v>
+      </c>
+      <c r="E77" s="1">
+        <f t="shared" ref="E77:F77" si="9">AVERAGE(E73:E76)</f>
+        <v>0.43514500000000006</v>
+      </c>
+      <c r="F77" s="1">
+        <f t="shared" si="9"/>
+        <v>0.28723937500000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>